<commit_message>
Changed excel sheet with plan for View Message Details page
</commit_message>
<xml_diff>
--- a/documents/connectbasket_info/ConnectBasketSpecifications.xlsx
+++ b/documents/connectbasket_info/ConnectBasketSpecifications.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\stak.engr.oregonstate.edu\Users\hellwegk\public_html\Capstone-2017-2018-Group-39\documents\connectbasket_info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{480E614F-7D4F-479C-ABDD-C4D925C26D90}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91FFA6A4-E7DD-4790-8FCC-A44441E521F4}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="5565" activeTab="1" xr2:uid="{935F0B6D-0491-44E1-9473-2B41384DF811}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="5565" activeTab="4" xr2:uid="{935F0B6D-0491-44E1-9473-2B41384DF811}"/>
   </bookViews>
   <sheets>
     <sheet name="CategoriesQuestions" sheetId="1" r:id="rId1"/>
     <sheet name="Groups" sheetId="2" r:id="rId2"/>
     <sheet name="Admin" sheetId="3" r:id="rId3"/>
     <sheet name="CreateMessageFields" sheetId="4" r:id="rId4"/>
+    <sheet name="View Message Details Fields" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="98">
   <si>
     <t>Type of Call</t>
   </si>
@@ -253,13 +254,82 @@
   </si>
   <si>
     <t>SA ORTHO TECHS</t>
+  </si>
+  <si>
+    <t>Fields to Go on View Message Details Page</t>
+  </si>
+  <si>
+    <t>Message Create Date</t>
+  </si>
+  <si>
+    <t>Patient</t>
+  </si>
+  <si>
+    <t>Owner</t>
+  </si>
+  <si>
+    <t>Owner Contact</t>
+  </si>
+  <si>
+    <t>Who</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Message/Note</t>
+  </si>
+  <si>
+    <t>Who Department</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Message/Notes Table</t>
+  </si>
+  <si>
+    <t>Add Note Button</t>
+  </si>
+  <si>
+    <t>Route To Input Box</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Routing History: </t>
+  </si>
+  <si>
+    <t>Routed To</t>
+  </si>
+  <si>
+    <t>Routed From</t>
+  </si>
+  <si>
+    <t>Mark as Completed Button</t>
+  </si>
+  <si>
+    <t>Message Created By</t>
+  </si>
+  <si>
+    <t>Message Created Department</t>
+  </si>
+  <si>
+    <t>Any info about patient?</t>
+  </si>
+  <si>
+    <t>Route Button</t>
+  </si>
+  <si>
+    <t>You can only see this if it is claimed by you</t>
+  </si>
+  <si>
+    <t>Claim Button for Unclaimed Messages/Unclaimed button for already claimed messages</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -273,13 +343,37 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -291,14 +385,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -733,7 +833,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B267644-D215-401E-BF0A-02CAA6F3F237}">
   <dimension ref="A1:A27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -1040,4 +1140,268 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6058BB96-5185-482A-AAC2-257E70320524}">
+  <dimension ref="A1:H31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="3"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>91</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>